<commit_message>
SUBIDA CON MODIFICACIÓN DEL HEADER
</commit_message>
<xml_diff>
--- a/TRABAJOS A REALIZAR.xlsx
+++ b/TRABAJOS A REALIZAR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DxOmega\Desktop\PAGINA-WEB-STAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1563CFA-98AF-4772-B4DD-86689576EE2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD49021-51FE-40ED-B4C7-93140497981C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="870" yWindow="3930" windowWidth="17625" windowHeight="15690" xr2:uid="{9F998DAA-B941-4C85-9B3A-20F7978CB856}"/>
   </bookViews>
@@ -103,18 +103,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -246,32 +241,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -285,6 +262,24 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -303,7 +298,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -331,11 +326,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -369,9 +364,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -433,14 +428,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="209549" cy="219076"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1034" name="Check Box 10" hidden="1">
@@ -449,7 +449,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBD82336-75BE-435C-A076-98C3375F00DF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -489,20 +489,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="209549" cy="219076"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1035" name="Check Box 11" hidden="1">
@@ -511,7 +516,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FCD55FA-99D5-4E4F-BABB-46911E69359A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -551,20 +556,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="209549" cy="219076"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1036" name="Check Box 12" hidden="1">
@@ -573,7 +583,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B3AF409-9085-472F-8225-07A3CAE7CF49}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -613,20 +623,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="209549" cy="219076"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1037" name="Check Box 13" hidden="1">
@@ -635,7 +650,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6DEC180-6014-4027-9ACF-432B6729A059}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -675,20 +690,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="209549" cy="219076"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1038" name="Check Box 14" hidden="1">
@@ -697,7 +717,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6968D62D-F2F7-46F5-B788-594CD3207E8D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -737,20 +757,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="209549" cy="219076"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1039" name="Check Box 15" hidden="1">
@@ -759,7 +784,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E88BDADB-8B90-4B43-BEC2-1B6A5D8B80F8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -799,20 +824,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="209549" cy="219076"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1040" name="Check Box 16" hidden="1">
@@ -821,7 +851,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15F4F85E-83A2-43F3-915B-21D956200D03}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -861,20 +891,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="209549" cy="219076"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
@@ -883,7 +918,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33814539-EC5C-42F6-8D27-D820468E5223}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -923,20 +958,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="209549" cy="219076"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
@@ -945,7 +985,7 @@
                   <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{107E8B60-24EE-491F-819E-7999682FB0FE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -985,20 +1025,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>20</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="209549" cy="219076"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
@@ -1007,7 +1052,7 @@
                   <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{426F3060-8C43-4F1E-A3E5-ECE5AD7358FF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1047,20 +1092,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="209549" cy="219076"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
@@ -1069,7 +1119,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCC12D13-0A55-41E1-A07C-2D2BC6AB0C28}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1109,20 +1159,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="209549" cy="219076"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1045" name="Check Box 21" hidden="1">
@@ -1131,7 +1186,7 @@
                   <a14:compatExt spid="_x0000_s1045"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C43FE46-55E3-4B4B-9A50-E600EECE9430}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1171,20 +1226,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="209549" cy="219076"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1046" name="Check Box 22" hidden="1">
@@ -1193,7 +1253,7 @@
                   <a14:compatExt spid="_x0000_s1046"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D125D7A5-5439-4953-A0BA-7253E198C782}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1233,20 +1293,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>295276</xdr:colOff>
+          <xdr:colOff>295275</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>180974</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="209549" cy="219076"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>504825</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1048" name="Check Box 24" hidden="1">
@@ -1255,7 +1320,7 @@
                   <a14:compatExt spid="_x0000_s1048"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A3948A3-228E-4C9F-BFC6-CAC49F31F24F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1295,7 +1360,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -1614,11 +1679,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1638,14 +1703,14 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4">
+      <c r="C3" s="2"/>
+      <c r="D3" s="18">
         <v>44232</v>
       </c>
       <c r="M3" t="s">
@@ -1653,156 +1718,156 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="19"/>
       <c r="M4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4">
+      <c r="C8" s="2"/>
+      <c r="D8" s="18">
         <v>44234</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="9"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="21"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="20"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4">
+      <c r="C14" s="2"/>
+      <c r="D14" s="18">
         <v>44236</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="9"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="21"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="9"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="21"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="9"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="10"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="22"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4">
+      <c r="C21" s="2"/>
+      <c r="D21" s="18">
         <v>44238</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="19"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="20"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">

</xml_diff>